<commit_message>
Latest Data Update Welsh & English
Latest Data Update Welsh & English
</commit_message>
<xml_diff>
--- a/cym/SOTD_QuestionAudit_Cymraeg_(SJ01).xlsx
+++ b/cym/SOTD_QuestionAudit_Cymraeg_(SJ01).xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -15384,55 +15385,49 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Mae ryg wedi'i wneud gan ddefnyddio ceinciau gwlân glas, porffor a choch yn unig. Mae </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+      <t xml:space="preserve">blue: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>x</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> o geinciau glas, pump gwaith yn fwy o geinciau porffor na cheinciau glas, ac 87 o geinciau coch yn llai na cheinciau porffor.
-O ystyried bod gan y ryg gyfanswm o 54 913 o geinciau gwlân, lluniwch hafaliad yn nhermau </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, purple: 5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
       </rPr>
       <t>x</t>
     </r>
     <r>
       <rPr>
         <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> a'i ddatrys i ganfod nifer y ceinciau gwlân glas yn y ryg.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">blue: </t>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, red: 5</t>
     </r>
     <r>
       <rPr>
@@ -15453,7 +15448,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, purple: 5</t>
+      <t xml:space="preserve"> – 87, </t>
     </r>
     <r>
       <rPr>
@@ -15474,7 +15469,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>, red: 5</t>
+      <t xml:space="preserve"> = 5000          If we add them all together they should equal 54913, </t>
     </r>
     <r>
       <rPr>
@@ -15495,7 +15490,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> – 87, </t>
+      <t xml:space="preserve"> + 5</t>
     </r>
     <r>
       <rPr>
@@ -15516,7 +15511,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> = 5000          If we add them all together they should equal 54913, </t>
+      <t xml:space="preserve"> + 5</t>
     </r>
     <r>
       <rPr>
@@ -15537,7 +15532,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> + 5</t>
+      <t xml:space="preserve"> – 87 = 54913, 11</t>
     </r>
     <r>
       <rPr>
@@ -15558,7 +15553,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> + 5</t>
+      <t xml:space="preserve"> – 87 = 54913, 11</t>
     </r>
     <r>
       <rPr>
@@ -15579,7 +15574,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> – 87 = 54913, 11</t>
+      <t xml:space="preserve"> = 55000, </t>
     </r>
     <r>
       <rPr>
@@ -15599,239 +15594,6 @@
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> – 87 = 54913, 11</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 55000, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> = 55000 ÷ 11</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">glas: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, porffor: 5</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>, coch: 5</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – 87, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = 5000          Os byddwn yn eu hadio i gyd at ei gilydd, dylen nhw fod yn hafal i 54913, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> + 5</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> + 5</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – 87 = 54913, 11</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> – 87 = 54913, 11</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> = 55000, </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>x</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = 55000 ÷ 11</t>
     </r>
@@ -17700,6 +17462,233 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> pensil?</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mae ryg wedi'i wneud gan ddefnyddio ceinciau gwlân glas, porffor a choch yn unig. Mae </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> o geinciau glas, pump gwaith yn fwy o geinciau porffor na cheinciau glas, ac 87 o geinciau coch yn llai na cheinciau porffor.
+O ystyried bod gan y ryg gyfanswm o 54 913 o geinciau gwlân, lluniwch hafaliad yn nhermau </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> a'i ddatrys i ganfod nifer y ceinciau gwlân glas yn y ryg.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">glas: </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, porffor: 5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>, coch: 5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – 87, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 5000          Os byddwn yn eu hadio i gyd at ei gilydd, dylen nhw fod yn hafal i 54913, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> + 5</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – 87 = 54913, 11</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> – 87 = 54913, 11</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 55000, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>x</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> = 55000 ÷ 11</t>
     </r>
   </si>
 </sst>
@@ -19339,8 +19328,8 @@
   <dimension ref="A1:I395"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D117" sqref="D117"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20123,10 +20112,10 @@
         <v>282</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>1775</v>
+        <v>1773</v>
       </c>
       <c r="F30" s="55" t="s">
-        <v>1776</v>
+        <v>1774</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>862</v>
@@ -20663,7 +20652,7 @@
         <v>808</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>1834</v>
+        <v>1832</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>46</v>
@@ -21417,7 +21406,7 @@
         <v>811</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>1835</v>
+        <v>1833</v>
       </c>
       <c r="D80" s="33" t="s">
         <v>68</v>
@@ -21943,10 +21932,10 @@
         <v>92</v>
       </c>
       <c r="E100" s="14" t="s">
-        <v>1777</v>
+        <v>1775</v>
       </c>
       <c r="F100" s="53" t="s">
-        <v>1778</v>
+        <v>1776</v>
       </c>
       <c r="G100" s="18" t="s">
         <v>935</v>
@@ -22540,7 +22529,7 @@
       <c r="C123" s="73" t="s">
         <v>742</v>
       </c>
-      <c r="D123" s="3" t="s">
+      <c r="D123" s="85" t="s">
         <v>123</v>
       </c>
       <c r="E123" s="44" t="s">
@@ -22696,7 +22685,7 @@
       <c r="C129" s="52" t="s">
         <v>1456</v>
       </c>
-      <c r="D129" s="3" t="s">
+      <c r="D129" s="85" t="s">
         <v>1539</v>
       </c>
       <c r="E129" s="13" t="s">
@@ -22722,7 +22711,7 @@
       <c r="C130" s="52" t="s">
         <v>1455</v>
       </c>
-      <c r="D130" s="3" t="s">
+      <c r="D130" s="85" t="s">
         <v>1541</v>
       </c>
       <c r="E130" s="13" t="s">
@@ -22823,7 +22812,7 @@
       <c r="C134" s="52" t="s">
         <v>552</v>
       </c>
-      <c r="D134" s="3" t="s">
+      <c r="D134" s="85" t="s">
         <v>970</v>
       </c>
       <c r="E134" s="13" t="s">
@@ -23103,7 +23092,7 @@
       <c r="B145" s="3" t="s">
         <v>831</v>
       </c>
-      <c r="C145" s="73" t="s">
+      <c r="C145" s="52" t="s">
         <v>637</v>
       </c>
       <c r="D145" s="3" t="s">
@@ -23207,7 +23196,7 @@
       <c r="B149" s="11" t="s">
         <v>136</v>
       </c>
-      <c r="C149" s="72" t="s">
+      <c r="C149" s="51" t="s">
         <v>638</v>
       </c>
       <c r="D149" s="11" t="s">
@@ -23340,7 +23329,7 @@
       <c r="C154" s="52" t="s">
         <v>1611</v>
       </c>
-      <c r="D154" s="3" t="s">
+      <c r="D154" s="85" t="s">
         <v>127</v>
       </c>
       <c r="E154" s="13">
@@ -23366,7 +23355,7 @@
       <c r="C155" s="52" t="s">
         <v>1611</v>
       </c>
-      <c r="D155" s="3" t="s">
+      <c r="D155" s="85" t="s">
         <v>128</v>
       </c>
       <c r="E155" s="13">
@@ -23597,7 +23586,7 @@
       <c r="B164" s="3" t="s">
         <v>1265</v>
       </c>
-      <c r="C164" s="73" t="s">
+      <c r="C164" s="52" t="s">
         <v>639</v>
       </c>
       <c r="D164" s="6" t="s">
@@ -23780,16 +23769,16 @@
         <v>820</v>
       </c>
       <c r="C171" s="54" t="s">
-        <v>1661</v>
+        <v>1834</v>
       </c>
       <c r="D171" s="33" t="s">
         <v>141</v>
       </c>
       <c r="E171" s="34" t="s">
-        <v>1662</v>
+        <v>1661</v>
       </c>
       <c r="F171" s="60" t="s">
-        <v>1663</v>
+        <v>1835</v>
       </c>
       <c r="G171" s="35" t="s">
         <v>1010</v>
@@ -23834,7 +23823,7 @@
       <c r="C173" s="52" t="s">
         <v>559</v>
       </c>
-      <c r="D173" s="3" t="s">
+      <c r="D173" s="85" t="s">
         <v>144</v>
       </c>
       <c r="E173" s="27">
@@ -23933,10 +23922,10 @@
         <v>129</v>
       </c>
       <c r="B177" s="6" t="s">
-        <v>1664</v>
+        <v>1662</v>
       </c>
       <c r="C177" s="56" t="s">
-        <v>1665</v>
+        <v>1663</v>
       </c>
       <c r="D177" s="6" t="s">
         <v>148</v>
@@ -23964,10 +23953,10 @@
         <v>149</v>
       </c>
       <c r="E178" s="14" t="s">
-        <v>1667</v>
+        <v>1665</v>
       </c>
       <c r="F178" s="53" t="s">
-        <v>1666</v>
+        <v>1664</v>
       </c>
       <c r="G178" s="18" t="s">
         <v>1016</v>
@@ -23990,10 +23979,10 @@
         <v>151</v>
       </c>
       <c r="E179" s="14" t="s">
-        <v>1669</v>
+        <v>1667</v>
       </c>
       <c r="F179" s="53" t="s">
-        <v>1668</v>
+        <v>1666</v>
       </c>
       <c r="G179" s="18" t="s">
         <v>1017</v>
@@ -24016,10 +24005,10 @@
         <v>63</v>
       </c>
       <c r="E180" s="13" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="F180" s="75" t="s">
-        <v>1670</v>
+        <v>1668</v>
       </c>
       <c r="G180" s="19" t="s">
         <v>1018</v>
@@ -24114,16 +24103,16 @@
         <v>157</v>
       </c>
       <c r="C184" s="52" t="s">
-        <v>1671</v>
+        <v>1669</v>
       </c>
       <c r="D184" s="3" t="s">
         <v>78</v>
       </c>
       <c r="E184" s="13" t="s">
-        <v>1672</v>
+        <v>1670</v>
       </c>
       <c r="F184" s="55" t="s">
-        <v>1673</v>
+        <v>1671</v>
       </c>
       <c r="G184" s="19" t="s">
         <v>1023</v>
@@ -24227,7 +24216,7 @@
         <v>1631</v>
       </c>
       <c r="F188" s="55" t="s">
-        <v>1674</v>
+        <v>1672</v>
       </c>
       <c r="G188" s="19" t="s">
         <v>1027</v>
@@ -24244,7 +24233,7 @@
         <v>1548</v>
       </c>
       <c r="C189" s="73" t="s">
-        <v>1675</v>
+        <v>1673</v>
       </c>
       <c r="D189" s="3" t="s">
         <v>77</v>
@@ -24267,10 +24256,10 @@
         <v>144</v>
       </c>
       <c r="B190" s="3" t="s">
-        <v>1676</v>
+        <v>1674</v>
       </c>
       <c r="C190" s="52" t="s">
-        <v>1677</v>
+        <v>1675</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>161</v>
@@ -24302,10 +24291,10 @@
         <v>163</v>
       </c>
       <c r="E191" s="42" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="F191" s="42" t="s">
-        <v>1678</v>
+        <v>1676</v>
       </c>
       <c r="G191" s="19" t="s">
         <v>1030</v>
@@ -24328,10 +24317,10 @@
         <v>164</v>
       </c>
       <c r="E192" s="43" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="F192" s="43" t="s">
-        <v>1679</v>
+        <v>1677</v>
       </c>
       <c r="G192" s="19" t="s">
         <v>1031</v>
@@ -24397,19 +24386,19 @@
         <v>148</v>
       </c>
       <c r="B195" s="33" t="s">
-        <v>1680</v>
+        <v>1678</v>
       </c>
       <c r="C195" s="54" t="s">
-        <v>1681</v>
+        <v>1679</v>
       </c>
       <c r="D195" s="33" t="s">
         <v>165</v>
       </c>
       <c r="E195" s="34" t="s">
-        <v>1682</v>
+        <v>1680</v>
       </c>
       <c r="F195" s="60" t="s">
-        <v>1683</v>
+        <v>1681</v>
       </c>
       <c r="G195" s="35" t="s">
         <v>1034</v>
@@ -24426,7 +24415,7 @@
         <v>166</v>
       </c>
       <c r="C196" s="52" t="s">
-        <v>1684</v>
+        <v>1682</v>
       </c>
       <c r="D196" s="3" t="s">
         <v>167</v>
@@ -24458,10 +24447,10 @@
         <v>1549</v>
       </c>
       <c r="E197" s="42" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="F197" s="42" t="s">
-        <v>1685</v>
+        <v>1683</v>
       </c>
       <c r="G197" s="19" t="s">
         <v>1036</v>
@@ -24475,10 +24464,10 @@
         <v>154</v>
       </c>
       <c r="B198" s="33" t="s">
-        <v>1686</v>
+        <v>1684</v>
       </c>
       <c r="C198" s="54" t="s">
-        <v>1687</v>
+        <v>1685</v>
       </c>
       <c r="D198" s="33" t="s">
         <v>77</v>
@@ -24504,7 +24493,7 @@
         <v>174</v>
       </c>
       <c r="C199" s="51" t="s">
-        <v>1688</v>
+        <v>1686</v>
       </c>
       <c r="D199" s="11" t="s">
         <v>175</v>
@@ -24513,7 +24502,7 @@
         <v>1315</v>
       </c>
       <c r="F199" s="53" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
       <c r="G199" s="18" t="s">
         <v>1038</v>
@@ -24530,7 +24519,7 @@
         <v>177</v>
       </c>
       <c r="C200" s="51" t="s">
-        <v>1690</v>
+        <v>1688</v>
       </c>
       <c r="D200" s="11" t="s">
         <v>176</v>
@@ -24671,10 +24660,10 @@
         <v>300</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>1691</v>
+        <v>1689</v>
       </c>
       <c r="C206" s="52" t="s">
-        <v>1692</v>
+        <v>1690</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>341</v>
@@ -24692,10 +24681,10 @@
         <v>301</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>1693</v>
+        <v>1691</v>
       </c>
       <c r="C207" s="52" t="s">
-        <v>1694</v>
+        <v>1692</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>342</v>
@@ -24713,7 +24702,7 @@
         <v>302</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1695</v>
+        <v>1693</v>
       </c>
       <c r="C208" s="52" t="s">
         <v>1586</v>
@@ -24781,7 +24770,7 @@
         <v>345</v>
       </c>
       <c r="C211" s="51" t="s">
-        <v>1696</v>
+        <v>1694</v>
       </c>
       <c r="D211" s="11" t="s">
         <v>347</v>
@@ -24821,7 +24810,7 @@
         <v>307</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1697</v>
+        <v>1695</v>
       </c>
       <c r="C213" s="52" t="s">
         <v>566</v>
@@ -25027,7 +25016,7 @@
         <v>185</v>
       </c>
       <c r="C221" s="51" t="s">
-        <v>1698</v>
+        <v>1696</v>
       </c>
       <c r="D221" s="11" t="s">
         <v>184</v>
@@ -25053,7 +25042,7 @@
         <v>186</v>
       </c>
       <c r="C222" s="51" t="s">
-        <v>1699</v>
+        <v>1697</v>
       </c>
       <c r="D222" s="11" t="s">
         <v>187</v>
@@ -25105,7 +25094,7 @@
         <v>191</v>
       </c>
       <c r="C224" s="54" t="s">
-        <v>1700</v>
+        <v>1698</v>
       </c>
       <c r="D224" s="33" t="s">
         <v>190</v>
@@ -25128,10 +25117,10 @@
         <v>166</v>
       </c>
       <c r="B225" s="3" t="s">
-        <v>1701</v>
+        <v>1699</v>
       </c>
       <c r="C225" s="52" t="s">
-        <v>1702</v>
+        <v>1700</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>24</v>
@@ -25183,16 +25172,16 @@
         <v>194</v>
       </c>
       <c r="C227" s="54" t="s">
-        <v>1703</v>
+        <v>1701</v>
       </c>
       <c r="D227" s="33" t="s">
         <v>193</v>
       </c>
       <c r="E227" s="34" t="s">
-        <v>1705</v>
+        <v>1703</v>
       </c>
       <c r="F227" s="60" t="s">
-        <v>1704</v>
+        <v>1702</v>
       </c>
       <c r="G227" s="35" t="s">
         <v>1067</v>
@@ -25206,10 +25195,10 @@
         <v>173</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="C228" s="52" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>77</v>
@@ -25267,10 +25256,10 @@
         <v>199</v>
       </c>
       <c r="E230" s="13" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
       <c r="F230" s="75" t="s">
-        <v>1708</v>
+        <v>1706</v>
       </c>
       <c r="G230" s="19" t="s">
         <v>1070</v>
@@ -25287,7 +25276,7 @@
         <v>354</v>
       </c>
       <c r="C231" s="51" t="s">
-        <v>1709</v>
+        <v>1707</v>
       </c>
       <c r="D231" s="11" t="s">
         <v>355</v>
@@ -25313,16 +25302,16 @@
         <v>1580</v>
       </c>
       <c r="C232" s="52" t="s">
-        <v>1710</v>
+        <v>1708</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>356</v>
       </c>
       <c r="E232" s="13" t="s">
-        <v>1711</v>
+        <v>1709</v>
       </c>
       <c r="F232" s="55" t="s">
-        <v>1712</v>
+        <v>1710</v>
       </c>
       <c r="G232" s="19" t="s">
         <v>1072</v>
@@ -25388,10 +25377,10 @@
         <v>316</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="C235" s="52" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>359</v>
@@ -25411,10 +25400,10 @@
         <v>317</v>
       </c>
       <c r="B236" s="3" t="s">
-        <v>1713</v>
+        <v>1711</v>
       </c>
       <c r="C236" s="52" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>452</v>
@@ -25486,7 +25475,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>1715</v>
+        <v>1713</v>
       </c>
       <c r="C239" s="52" t="s">
         <v>572</v>
@@ -25495,10 +25484,10 @@
         <v>200</v>
       </c>
       <c r="E239" s="13" t="s">
-        <v>1716</v>
+        <v>1714</v>
       </c>
       <c r="F239" s="55" t="s">
-        <v>1717</v>
+        <v>1715</v>
       </c>
       <c r="G239" s="19" t="s">
         <v>1079</v>
@@ -25524,7 +25513,7 @@
         <v>516</v>
       </c>
       <c r="F240" s="55" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
       <c r="G240" s="19" t="s">
         <v>1080</v>
@@ -25564,10 +25553,10 @@
         <v>177</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
       <c r="C242" s="52" t="s">
-        <v>1720</v>
+        <v>1718</v>
       </c>
       <c r="D242" s="6" t="s">
         <v>24</v>
@@ -25590,10 +25579,10 @@
         <v>178</v>
       </c>
       <c r="B243" s="33" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
       <c r="C243" s="54" t="s">
-        <v>1722</v>
+        <v>1720</v>
       </c>
       <c r="D243" s="33" t="s">
         <v>204</v>
@@ -25619,7 +25608,7 @@
         <v>361</v>
       </c>
       <c r="C244" s="51" t="s">
-        <v>1723</v>
+        <v>1721</v>
       </c>
       <c r="D244" s="11" t="s">
         <v>1084</v>
@@ -25671,7 +25660,7 @@
         <v>1231</v>
       </c>
       <c r="C246" s="54" t="s">
-        <v>1725</v>
+        <v>1723</v>
       </c>
       <c r="D246" s="33" t="s">
         <v>369</v>
@@ -25723,16 +25712,16 @@
         <v>1485</v>
       </c>
       <c r="C248" s="54" t="s">
-        <v>1726</v>
+        <v>1724</v>
       </c>
       <c r="D248" s="33" t="s">
         <v>371</v>
       </c>
       <c r="E248" s="34" t="s">
-        <v>1727</v>
+        <v>1725</v>
       </c>
       <c r="F248" s="60" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
       <c r="G248" s="35" t="s">
         <v>1089</v>
@@ -25749,7 +25738,7 @@
         <v>1232</v>
       </c>
       <c r="C249" s="51" t="s">
-        <v>1729</v>
+        <v>1727</v>
       </c>
       <c r="D249" s="11" t="s">
         <v>114</v>
@@ -25915,10 +25904,10 @@
         <v>188</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>1730</v>
+        <v>1728</v>
       </c>
       <c r="C256" s="52" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
       <c r="D256" s="3" t="s">
         <v>63</v>
@@ -25970,16 +25959,16 @@
         <v>216</v>
       </c>
       <c r="C258" s="52" t="s">
-        <v>1732</v>
+        <v>1730</v>
       </c>
       <c r="D258" s="3" t="s">
         <v>217</v>
       </c>
       <c r="E258" s="13" t="s">
-        <v>1733</v>
+        <v>1731</v>
       </c>
       <c r="F258" s="55" t="s">
-        <v>1734</v>
+        <v>1732</v>
       </c>
       <c r="G258" s="19" t="s">
         <v>1099</v>
@@ -26002,10 +25991,10 @@
         <v>63</v>
       </c>
       <c r="E259" s="13" t="s">
-        <v>1735</v>
+        <v>1733</v>
       </c>
       <c r="F259" s="75" t="s">
-        <v>1736</v>
+        <v>1734</v>
       </c>
       <c r="G259" s="19" t="s">
         <v>1100</v>
@@ -26019,10 +26008,10 @@
         <v>192</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
       <c r="C260" s="52" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D260" s="3" t="s">
         <v>1101</v>
@@ -26048,7 +26037,7 @@
         <v>1235</v>
       </c>
       <c r="C261" s="52" t="s">
-        <v>1737</v>
+        <v>1735</v>
       </c>
       <c r="D261" s="3" t="s">
         <v>218</v>
@@ -26132,10 +26121,10 @@
         <v>206</v>
       </c>
       <c r="E264" s="14" t="s">
-        <v>1738</v>
+        <v>1736</v>
       </c>
       <c r="F264" s="84" t="s">
-        <v>1739</v>
+        <v>1737</v>
       </c>
       <c r="G264" s="18" t="s">
         <v>1106</v>
@@ -26152,7 +26141,7 @@
         <v>1107</v>
       </c>
       <c r="C265" s="51" t="s">
-        <v>1740</v>
+        <v>1738</v>
       </c>
       <c r="D265" s="11" t="s">
         <v>207</v>
@@ -26178,7 +26167,7 @@
         <v>1109</v>
       </c>
       <c r="C266" s="51" t="s">
-        <v>1741</v>
+        <v>1739</v>
       </c>
       <c r="D266" s="11" t="s">
         <v>207</v>
@@ -26227,10 +26216,10 @@
         <v>183</v>
       </c>
       <c r="B268" s="3" t="s">
-        <v>1742</v>
+        <v>1740</v>
       </c>
       <c r="C268" s="52" t="s">
-        <v>1743</v>
+        <v>1741</v>
       </c>
       <c r="D268" s="6" t="s">
         <v>24</v>
@@ -26494,7 +26483,7 @@
         <v>460</v>
       </c>
       <c r="F278" s="53" t="s">
-        <v>1744</v>
+        <v>1742</v>
       </c>
       <c r="G278" s="18" t="s">
         <v>1122</v>
@@ -26543,10 +26532,10 @@
         <v>380</v>
       </c>
       <c r="E280" s="14" t="s">
-        <v>1745</v>
+        <v>1743</v>
       </c>
       <c r="F280" s="53" t="s">
-        <v>1746</v>
+        <v>1744</v>
       </c>
       <c r="G280" s="18" t="s">
         <v>1125</v>
@@ -26637,7 +26626,7 @@
         <v>386</v>
       </c>
       <c r="C284" s="51" t="s">
-        <v>1747</v>
+        <v>1745</v>
       </c>
       <c r="D284" s="11" t="s">
         <v>387</v>
@@ -26663,7 +26652,7 @@
         <v>1243</v>
       </c>
       <c r="C285" s="51" t="s">
-        <v>1748</v>
+        <v>1746</v>
       </c>
       <c r="D285" s="11" t="s">
         <v>355</v>
@@ -26689,7 +26678,7 @@
         <v>388</v>
       </c>
       <c r="C286" s="51" t="s">
-        <v>1749</v>
+        <v>1747</v>
       </c>
       <c r="D286" s="11" t="s">
         <v>382</v>
@@ -26741,7 +26730,7 @@
         <v>373</v>
       </c>
       <c r="C288" s="56" t="s">
-        <v>1750</v>
+        <v>1748</v>
       </c>
       <c r="D288" s="6"/>
       <c r="E288" s="23"/>
@@ -26761,7 +26750,7 @@
         <v>390</v>
       </c>
       <c r="C289" s="54" t="s">
-        <v>1751</v>
+        <v>1749</v>
       </c>
       <c r="D289" s="33" t="s">
         <v>391</v>
@@ -26822,7 +26811,7 @@
         <v>1564</v>
       </c>
       <c r="F291" s="53" t="s">
-        <v>1752</v>
+        <v>1750</v>
       </c>
       <c r="G291" s="18" t="s">
         <v>1137</v>
@@ -26865,7 +26854,7 @@
         <v>1245</v>
       </c>
       <c r="C293" s="54" t="s">
-        <v>1753</v>
+        <v>1751</v>
       </c>
       <c r="D293" s="33" t="s">
         <v>223</v>
@@ -26917,16 +26906,16 @@
         <v>1581</v>
       </c>
       <c r="C295" s="54" t="s">
-        <v>1754</v>
+        <v>1752</v>
       </c>
       <c r="D295" s="33" t="s">
         <v>221</v>
       </c>
       <c r="E295" s="34" t="s">
-        <v>1755</v>
+        <v>1753</v>
       </c>
       <c r="F295" s="60" t="s">
-        <v>1756</v>
+        <v>1754</v>
       </c>
       <c r="G295" s="35" t="s">
         <v>1141</v>
@@ -26995,7 +26984,7 @@
         <v>1246</v>
       </c>
       <c r="C298" s="54" t="s">
-        <v>1757</v>
+        <v>1755</v>
       </c>
       <c r="D298" s="33" t="s">
         <v>395</v>
@@ -27047,7 +27036,7 @@
         <v>1248</v>
       </c>
       <c r="C300" s="54" t="s">
-        <v>1758</v>
+        <v>1756</v>
       </c>
       <c r="D300" s="33" t="s">
         <v>397</v>
@@ -27257,10 +27246,10 @@
         <v>77</v>
       </c>
       <c r="E308" s="13" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="F308" s="75" t="s">
-        <v>1759</v>
+        <v>1757</v>
       </c>
       <c r="G308" s="19" t="s">
         <v>1154</v>
@@ -27378,19 +27367,19 @@
         <v>202</v>
       </c>
       <c r="B313" s="33" t="s">
-        <v>1760</v>
+        <v>1758</v>
       </c>
       <c r="C313" s="54" t="s">
-        <v>1761</v>
+        <v>1759</v>
       </c>
       <c r="D313" s="33" t="s">
         <v>224</v>
       </c>
       <c r="E313" s="34" t="s">
-        <v>1790</v>
+        <v>1788</v>
       </c>
       <c r="F313" s="60" t="s">
-        <v>1791</v>
+        <v>1789</v>
       </c>
       <c r="G313" s="35" t="s">
         <v>1159</v>
@@ -27413,10 +27402,10 @@
         <v>226</v>
       </c>
       <c r="E314" s="14" t="s">
-        <v>1762</v>
+        <v>1760</v>
       </c>
       <c r="F314" s="53" t="s">
-        <v>1763</v>
+        <v>1761</v>
       </c>
       <c r="G314" s="18" t="s">
         <v>1160</v>
@@ -27618,10 +27607,10 @@
         <v>366</v>
       </c>
       <c r="B322" s="33" t="s">
-        <v>1765</v>
+        <v>1763</v>
       </c>
       <c r="C322" s="54" t="s">
-        <v>1764</v>
+        <v>1762</v>
       </c>
       <c r="D322" s="33" t="s">
         <v>355</v>
@@ -27725,7 +27714,7 @@
         <v>431</v>
       </c>
       <c r="C326" s="52" t="s">
-        <v>1766</v>
+        <v>1764</v>
       </c>
       <c r="D326" s="3" t="s">
         <v>406</v>
@@ -27855,7 +27844,7 @@
         <v>426</v>
       </c>
       <c r="C331" s="54" t="s">
-        <v>1767</v>
+        <v>1765</v>
       </c>
       <c r="D331" s="33" t="s">
         <v>427</v>
@@ -27890,7 +27879,7 @@
         <v>476</v>
       </c>
       <c r="F332" s="63" t="s">
-        <v>1768</v>
+        <v>1766</v>
       </c>
       <c r="G332" s="19" t="s">
         <v>1179</v>
@@ -27930,7 +27919,7 @@
         <v>370</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1769</v>
+        <v>1767</v>
       </c>
       <c r="C334" s="52" t="s">
         <v>1622</v>
@@ -28013,10 +28002,10 @@
         <v>24</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="F337" s="55" t="s">
-        <v>1770</v>
+        <v>1768</v>
       </c>
       <c r="G337" s="19" t="s">
         <v>1184</v>
@@ -28056,10 +28045,10 @@
         <v>219</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1786</v>
+        <v>1784</v>
       </c>
       <c r="C339" s="52" t="s">
-        <v>1714</v>
+        <v>1712</v>
       </c>
       <c r="D339" s="3" t="s">
         <v>238</v>
@@ -28082,19 +28071,19 @@
         <v>211</v>
       </c>
       <c r="B340" s="33" t="s">
-        <v>1771</v>
+        <v>1769</v>
       </c>
       <c r="C340" s="54" t="s">
-        <v>1772</v>
+        <v>1770</v>
       </c>
       <c r="D340" s="33" t="s">
         <v>231</v>
       </c>
       <c r="E340" s="34" t="s">
-        <v>1792</v>
+        <v>1790</v>
       </c>
       <c r="F340" s="60" t="s">
-        <v>1793</v>
+        <v>1791</v>
       </c>
       <c r="G340" s="35" t="s">
         <v>1187</v>
@@ -28117,10 +28106,10 @@
         <v>232</v>
       </c>
       <c r="E341" s="34" t="s">
-        <v>1773</v>
+        <v>1771</v>
       </c>
       <c r="F341" s="60" t="s">
-        <v>1774</v>
+        <v>1772</v>
       </c>
       <c r="G341" s="35" t="s">
         <v>1188</v>
@@ -28143,10 +28132,10 @@
         <v>114</v>
       </c>
       <c r="E342" s="34" t="s">
-        <v>1779</v>
+        <v>1777</v>
       </c>
       <c r="F342" s="60" t="s">
-        <v>1780</v>
+        <v>1778</v>
       </c>
       <c r="G342" s="35" t="s">
         <v>1189</v>
@@ -28189,7 +28178,7 @@
         <v>234</v>
       </c>
       <c r="C344" s="52" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="D344" s="3" t="s">
         <v>1569</v>
@@ -28221,10 +28210,10 @@
         <v>1572</v>
       </c>
       <c r="E345" s="42" t="s">
-        <v>1782</v>
+        <v>1780</v>
       </c>
       <c r="F345" s="78" t="s">
-        <v>1783</v>
+        <v>1781</v>
       </c>
       <c r="G345" s="19" t="s">
         <v>1192</v>
@@ -28241,7 +28230,7 @@
         <v>432</v>
       </c>
       <c r="C346" s="52" t="s">
-        <v>1784</v>
+        <v>1782</v>
       </c>
       <c r="D346" s="3" t="s">
         <v>406</v>
@@ -28267,7 +28256,7 @@
         <v>1259</v>
       </c>
       <c r="C347" s="52" t="s">
-        <v>1785</v>
+        <v>1783</v>
       </c>
       <c r="D347" s="3" t="s">
         <v>433</v>
@@ -28345,7 +28334,7 @@
         <v>240</v>
       </c>
       <c r="C350" s="52" t="s">
-        <v>1787</v>
+        <v>1785</v>
       </c>
       <c r="D350" s="3" t="s">
         <v>241</v>
@@ -28394,19 +28383,19 @@
         <v>222</v>
       </c>
       <c r="B352" s="33" t="s">
-        <v>1788</v>
+        <v>1786</v>
       </c>
       <c r="C352" s="54" t="s">
-        <v>1789</v>
+        <v>1787</v>
       </c>
       <c r="D352" s="33" t="s">
         <v>243</v>
       </c>
       <c r="E352" s="34" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="F352" s="60" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="G352" s="35" t="s">
         <v>1199</v>
@@ -28429,10 +28418,10 @@
         <v>245</v>
       </c>
       <c r="E353" s="34" t="s">
-        <v>1796</v>
+        <v>1794</v>
       </c>
       <c r="F353" s="60" t="s">
-        <v>1797</v>
+        <v>1795</v>
       </c>
       <c r="G353" s="35" t="s">
         <v>1200</v>
@@ -28468,10 +28457,10 @@
         <v>225</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>1799</v>
+        <v>1797</v>
       </c>
       <c r="C355" s="52" t="s">
-        <v>1798</v>
+        <v>1796</v>
       </c>
       <c r="D355" s="3" t="s">
         <v>247</v>
@@ -28503,10 +28492,10 @@
         <v>1136</v>
       </c>
       <c r="E356" s="34" t="s">
-        <v>1800</v>
+        <v>1798</v>
       </c>
       <c r="F356" s="60" t="s">
-        <v>1801</v>
+        <v>1799</v>
       </c>
       <c r="G356" s="35" t="s">
         <v>1203</v>
@@ -28523,7 +28512,7 @@
         <v>234</v>
       </c>
       <c r="C357" s="52" t="s">
-        <v>1781</v>
+        <v>1779</v>
       </c>
       <c r="D357" s="3" t="s">
         <v>1573</v>
@@ -28546,7 +28535,7 @@
         <v>229</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>1802</v>
+        <v>1800</v>
       </c>
       <c r="C358" s="52" t="s">
         <v>741</v>
@@ -28572,7 +28561,7 @@
         <v>232</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1803</v>
+        <v>1801</v>
       </c>
       <c r="C359" s="52" t="s">
         <v>741</v>
@@ -28612,7 +28601,7 @@
         <v>1207</v>
       </c>
       <c r="H360" t="s">
-        <v>1804</v>
+        <v>1802</v>
       </c>
     </row>
     <row r="361" spans="1:8" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -28629,10 +28618,10 @@
         <v>114</v>
       </c>
       <c r="E361" s="34" t="s">
-        <v>1805</v>
+        <v>1803</v>
       </c>
       <c r="F361" s="60" t="s">
-        <v>1806</v>
+        <v>1804</v>
       </c>
       <c r="G361" s="35" t="s">
         <v>1208</v>
@@ -28675,16 +28664,16 @@
         <v>274</v>
       </c>
       <c r="C363" s="54" t="s">
-        <v>1807</v>
+        <v>1805</v>
       </c>
       <c r="D363" s="33" t="s">
         <v>275</v>
       </c>
       <c r="E363" s="34" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="F363" s="60" t="s">
-        <v>1808</v>
+        <v>1806</v>
       </c>
       <c r="G363" s="35" t="s">
         <v>1210</v>
@@ -28707,10 +28696,10 @@
         <v>277</v>
       </c>
       <c r="E364" s="34" t="s">
-        <v>1809</v>
+        <v>1807</v>
       </c>
       <c r="F364" s="60" t="s">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="G364" s="35" t="s">
         <v>1211</v>
@@ -28724,19 +28713,19 @@
         <v>234</v>
       </c>
       <c r="B365" s="33" t="s">
-        <v>1811</v>
+        <v>1809</v>
       </c>
       <c r="C365" s="54" t="s">
-        <v>1812</v>
+        <v>1810</v>
       </c>
       <c r="D365" s="33" t="s">
         <v>255</v>
       </c>
       <c r="E365" s="34" t="s">
-        <v>1794</v>
+        <v>1792</v>
       </c>
       <c r="F365" s="60" t="s">
-        <v>1795</v>
+        <v>1793</v>
       </c>
       <c r="G365" s="35" t="s">
         <v>1212</v>
@@ -28759,10 +28748,10 @@
         <v>114</v>
       </c>
       <c r="E366" s="34" t="s">
-        <v>1813</v>
+        <v>1811</v>
       </c>
       <c r="F366" s="60" t="s">
-        <v>1814</v>
+        <v>1812</v>
       </c>
       <c r="G366" s="35" t="s">
         <v>1213</v>
@@ -28801,16 +28790,16 @@
         <v>258</v>
       </c>
       <c r="C368" s="54" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
       <c r="D368" s="33" t="s">
         <v>1136</v>
       </c>
       <c r="E368" s="34" t="s">
-        <v>1815</v>
+        <v>1813</v>
       </c>
       <c r="F368" s="60" t="s">
-        <v>1816</v>
+        <v>1814</v>
       </c>
       <c r="G368" s="35" t="s">
         <v>1215</v>
@@ -28833,10 +28822,10 @@
         <v>260</v>
       </c>
       <c r="E369" s="34" t="s">
-        <v>1817</v>
+        <v>1815</v>
       </c>
       <c r="F369" s="76" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
       <c r="G369" s="35" t="s">
         <v>1216</v>
@@ -28879,16 +28868,16 @@
         <v>262</v>
       </c>
       <c r="C371" s="52" t="s">
-        <v>1819</v>
+        <v>1817</v>
       </c>
       <c r="D371" s="3" t="s">
         <v>263</v>
       </c>
       <c r="E371" s="13" t="s">
-        <v>1820</v>
+        <v>1818</v>
       </c>
       <c r="F371" s="55" t="s">
-        <v>1821</v>
+        <v>1819</v>
       </c>
       <c r="G371" s="19" t="s">
         <v>1218</v>
@@ -28937,10 +28926,10 @@
         <v>267</v>
       </c>
       <c r="E373" s="13" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="F373" s="55" t="s">
-        <v>1822</v>
+        <v>1820</v>
       </c>
       <c r="G373" s="19" t="s">
         <v>1220</v>
@@ -28954,19 +28943,19 @@
         <v>245</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1824</v>
+        <v>1822</v>
       </c>
       <c r="C374" s="52" t="s">
-        <v>1823</v>
+        <v>1821</v>
       </c>
       <c r="D374" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E374" s="13" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="F374" s="55" t="s">
-        <v>1825</v>
+        <v>1823</v>
       </c>
       <c r="G374" s="19" t="s">
         <v>1221</v>
@@ -29009,7 +28998,7 @@
         <v>1262</v>
       </c>
       <c r="C376" s="54" t="s">
-        <v>1826</v>
+        <v>1824</v>
       </c>
       <c r="D376" s="33" t="s">
         <v>266</v>
@@ -29035,7 +29024,7 @@
         <v>270</v>
       </c>
       <c r="C377" s="52" t="s">
-        <v>1827</v>
+        <v>1825</v>
       </c>
       <c r="D377" s="3" t="s">
         <v>268</v>
@@ -29061,7 +29050,7 @@
         <v>271</v>
       </c>
       <c r="C378" s="52" t="s">
-        <v>1828</v>
+        <v>1826</v>
       </c>
       <c r="D378" s="3" t="s">
         <v>269</v>
@@ -29087,7 +29076,7 @@
         <v>272</v>
       </c>
       <c r="C379" s="52" t="s">
-        <v>1829</v>
+        <v>1827</v>
       </c>
       <c r="D379" s="3" t="s">
         <v>273</v>
@@ -29110,19 +29099,19 @@
         <v>249</v>
       </c>
       <c r="B380" s="33" t="s">
-        <v>1830</v>
+        <v>1828</v>
       </c>
       <c r="C380" s="54" t="s">
-        <v>1833</v>
+        <v>1831</v>
       </c>
       <c r="D380" s="33" t="s">
         <v>338</v>
       </c>
       <c r="E380" s="34" t="s">
-        <v>1831</v>
+        <v>1829</v>
       </c>
       <c r="F380" s="60" t="s">
-        <v>1832</v>
+        <v>1830</v>
       </c>
       <c r="G380" s="35" t="s">
         <v>1227</v>

</xml_diff>

<commit_message>
latest Data Translation Update
latest Data Translation Update
</commit_message>
<xml_diff>
--- a/cym/SOTD_QuestionAudit_Cymraeg_(SJ01).xlsx
+++ b/cym/SOTD_QuestionAudit_Cymraeg_(SJ01).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="120" windowWidth="18750" windowHeight="11640"/>
+    <workbookView xWindow="-1800" yWindow="1470" windowWidth="18750" windowHeight="11580"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -15736,35 +15735,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Ysgrifennwch </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>n</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>fed term y dilyniant uchod.</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>7 × 10</t>
     </r>
     <r>
@@ -17689,6 +17659,29 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> = 55000 ÷ 11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ysgrifennwch </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>n</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>fed term y dilyniant uchod.</t>
     </r>
   </si>
 </sst>
@@ -19328,8 +19321,8 @@
   <dimension ref="A1:I395"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D173" sqref="D173"/>
+      <pane ySplit="1" topLeftCell="A214" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D223" sqref="D223"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20112,10 +20105,10 @@
         <v>282</v>
       </c>
       <c r="E30" s="13" t="s">
+        <v>1772</v>
+      </c>
+      <c r="F30" s="55" t="s">
         <v>1773</v>
-      </c>
-      <c r="F30" s="55" t="s">
-        <v>1774</v>
       </c>
       <c r="G30" s="19" t="s">
         <v>862</v>
@@ -20652,7 +20645,7 @@
         <v>808</v>
       </c>
       <c r="C51" s="52" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>46</v>
@@ -21406,7 +21399,7 @@
         <v>811</v>
       </c>
       <c r="C80" s="54" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D80" s="33" t="s">
         <v>68</v>
@@ -21932,10 +21925,10 @@
         <v>92</v>
       </c>
       <c r="E100" s="14" t="s">
+        <v>1774</v>
+      </c>
+      <c r="F100" s="53" t="s">
         <v>1775</v>
-      </c>
-      <c r="F100" s="53" t="s">
-        <v>1776</v>
       </c>
       <c r="G100" s="18" t="s">
         <v>935</v>
@@ -23769,7 +23762,7 @@
         <v>820</v>
       </c>
       <c r="C171" s="54" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D171" s="33" t="s">
         <v>141</v>
@@ -23778,7 +23771,7 @@
         <v>1661</v>
       </c>
       <c r="F171" s="60" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="G171" s="35" t="s">
         <v>1010</v>
@@ -24154,7 +24147,7 @@
       <c r="B186" s="3" t="s">
         <v>822</v>
       </c>
-      <c r="C186" s="73" t="s">
+      <c r="C186" s="52" t="s">
         <v>751</v>
       </c>
       <c r="D186" s="3" t="s">
@@ -24206,7 +24199,7 @@
       <c r="B188" s="3" t="s">
         <v>823</v>
       </c>
-      <c r="C188" s="73" t="s">
+      <c r="C188" s="52" t="s">
         <v>753</v>
       </c>
       <c r="D188" t="s">
@@ -24259,7 +24252,7 @@
         <v>1674</v>
       </c>
       <c r="C190" s="52" t="s">
-        <v>1675</v>
+        <v>1835</v>
       </c>
       <c r="D190" s="3" t="s">
         <v>161</v>
@@ -24291,10 +24284,10 @@
         <v>163</v>
       </c>
       <c r="E191" s="42" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="F191" s="42" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="G191" s="19" t="s">
         <v>1030</v>
@@ -24317,10 +24310,10 @@
         <v>164</v>
       </c>
       <c r="E192" s="43" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="F192" s="43" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="G192" s="19" t="s">
         <v>1031</v>
@@ -24386,19 +24379,19 @@
         <v>148</v>
       </c>
       <c r="B195" s="33" t="s">
+        <v>1677</v>
+      </c>
+      <c r="C195" s="54" t="s">
         <v>1678</v>
-      </c>
-      <c r="C195" s="54" t="s">
-        <v>1679</v>
       </c>
       <c r="D195" s="33" t="s">
         <v>165</v>
       </c>
       <c r="E195" s="34" t="s">
+        <v>1679</v>
+      </c>
+      <c r="F195" s="60" t="s">
         <v>1680</v>
-      </c>
-      <c r="F195" s="60" t="s">
-        <v>1681</v>
       </c>
       <c r="G195" s="35" t="s">
         <v>1034</v>
@@ -24415,9 +24408,9 @@
         <v>166</v>
       </c>
       <c r="C196" s="52" t="s">
-        <v>1682</v>
-      </c>
-      <c r="D196" s="3" t="s">
+        <v>1681</v>
+      </c>
+      <c r="D196" s="85" t="s">
         <v>167</v>
       </c>
       <c r="E196" s="27">
@@ -24443,14 +24436,14 @@
       <c r="C197" s="52" t="s">
         <v>527</v>
       </c>
-      <c r="D197" s="3" t="s">
+      <c r="D197" s="85" t="s">
         <v>1549</v>
       </c>
       <c r="E197" s="42" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="F197" s="42" t="s">
-        <v>1683</v>
+        <v>1682</v>
       </c>
       <c r="G197" s="19" t="s">
         <v>1036</v>
@@ -24464,10 +24457,10 @@
         <v>154</v>
       </c>
       <c r="B198" s="33" t="s">
+        <v>1683</v>
+      </c>
+      <c r="C198" s="54" t="s">
         <v>1684</v>
-      </c>
-      <c r="C198" s="54" t="s">
-        <v>1685</v>
       </c>
       <c r="D198" s="33" t="s">
         <v>77</v>
@@ -24493,7 +24486,7 @@
         <v>174</v>
       </c>
       <c r="C199" s="51" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D199" s="11" t="s">
         <v>175</v>
@@ -24502,7 +24495,7 @@
         <v>1315</v>
       </c>
       <c r="F199" s="53" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="G199" s="18" t="s">
         <v>1038</v>
@@ -24519,7 +24512,7 @@
         <v>177</v>
       </c>
       <c r="C200" s="51" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D200" s="11" t="s">
         <v>176</v>
@@ -24544,10 +24537,10 @@
       <c r="B201" s="3" t="s">
         <v>825</v>
       </c>
-      <c r="C201" s="73" t="s">
+      <c r="C201" s="52" t="s">
         <v>643</v>
       </c>
-      <c r="D201" s="3" t="s">
+      <c r="D201" s="85" t="s">
         <v>171</v>
       </c>
       <c r="E201" s="44" t="s">
@@ -24570,7 +24563,7 @@
       <c r="B202" s="3" t="s">
         <v>824</v>
       </c>
-      <c r="C202" s="73" t="s">
+      <c r="C202" s="52" t="s">
         <v>642</v>
       </c>
       <c r="D202" s="3" t="s">
@@ -24660,10 +24653,10 @@
         <v>300</v>
       </c>
       <c r="B206" s="3" t="s">
+        <v>1688</v>
+      </c>
+      <c r="C206" s="52" t="s">
         <v>1689</v>
-      </c>
-      <c r="C206" s="52" t="s">
-        <v>1690</v>
       </c>
       <c r="D206" s="3" t="s">
         <v>341</v>
@@ -24681,10 +24674,10 @@
         <v>301</v>
       </c>
       <c r="B207" s="3" t="s">
+        <v>1690</v>
+      </c>
+      <c r="C207" s="52" t="s">
         <v>1691</v>
-      </c>
-      <c r="C207" s="52" t="s">
-        <v>1692</v>
       </c>
       <c r="D207" s="3" t="s">
         <v>342</v>
@@ -24702,12 +24695,12 @@
         <v>302</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="C208" s="52" t="s">
         <v>1586</v>
       </c>
-      <c r="D208" s="3" t="s">
+      <c r="D208" s="85" t="s">
         <v>343</v>
       </c>
       <c r="F208" s="13"/>
@@ -24770,7 +24763,7 @@
         <v>345</v>
       </c>
       <c r="C211" s="51" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D211" s="11" t="s">
         <v>347</v>
@@ -24810,7 +24803,7 @@
         <v>307</v>
       </c>
       <c r="B213" s="3" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="C213" s="52" t="s">
         <v>566</v>
@@ -25016,7 +25009,7 @@
         <v>185</v>
       </c>
       <c r="C221" s="51" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D221" s="11" t="s">
         <v>184</v>
@@ -25042,7 +25035,7 @@
         <v>186</v>
       </c>
       <c r="C222" s="51" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D222" s="11" t="s">
         <v>187</v>
@@ -25070,7 +25063,7 @@
       <c r="C223" s="52" t="s">
         <v>571</v>
       </c>
-      <c r="D223" s="3" t="s">
+      <c r="D223" s="85" t="s">
         <v>188</v>
       </c>
       <c r="E223" s="13" t="s">
@@ -25094,7 +25087,7 @@
         <v>191</v>
       </c>
       <c r="C224" s="54" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D224" s="33" t="s">
         <v>190</v>
@@ -25117,10 +25110,10 @@
         <v>166</v>
       </c>
       <c r="B225" s="3" t="s">
+        <v>1698</v>
+      </c>
+      <c r="C225" s="52" t="s">
         <v>1699</v>
-      </c>
-      <c r="C225" s="52" t="s">
-        <v>1700</v>
       </c>
       <c r="D225" s="6" t="s">
         <v>24</v>
@@ -25172,16 +25165,16 @@
         <v>194</v>
       </c>
       <c r="C227" s="54" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D227" s="33" t="s">
         <v>193</v>
       </c>
       <c r="E227" s="34" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="F227" s="60" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="G227" s="35" t="s">
         <v>1067</v>
@@ -25195,10 +25188,10 @@
         <v>173</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="C228" s="52" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D228" s="3" t="s">
         <v>77</v>
@@ -25256,10 +25249,10 @@
         <v>199</v>
       </c>
       <c r="E230" s="13" t="s">
+        <v>1704</v>
+      </c>
+      <c r="F230" s="75" t="s">
         <v>1705</v>
-      </c>
-      <c r="F230" s="75" t="s">
-        <v>1706</v>
       </c>
       <c r="G230" s="19" t="s">
         <v>1070</v>
@@ -25276,7 +25269,7 @@
         <v>354</v>
       </c>
       <c r="C231" s="51" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D231" s="11" t="s">
         <v>355</v>
@@ -25302,16 +25295,16 @@
         <v>1580</v>
       </c>
       <c r="C232" s="52" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D232" s="3" t="s">
         <v>356</v>
       </c>
       <c r="E232" s="13" t="s">
+        <v>1708</v>
+      </c>
+      <c r="F232" s="55" t="s">
         <v>1709</v>
-      </c>
-      <c r="F232" s="55" t="s">
-        <v>1710</v>
       </c>
       <c r="G232" s="19" t="s">
         <v>1072</v>
@@ -25377,10 +25370,10 @@
         <v>316</v>
       </c>
       <c r="B235" s="3" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C235" s="52" t="s">
         <v>1711</v>
-      </c>
-      <c r="C235" s="52" t="s">
-        <v>1712</v>
       </c>
       <c r="D235" s="3" t="s">
         <v>359</v>
@@ -25400,10 +25393,10 @@
         <v>317</v>
       </c>
       <c r="B236" s="3" t="s">
+        <v>1710</v>
+      </c>
+      <c r="C236" s="52" t="s">
         <v>1711</v>
-      </c>
-      <c r="C236" s="52" t="s">
-        <v>1712</v>
       </c>
       <c r="D236" s="3" t="s">
         <v>452</v>
@@ -25475,7 +25468,7 @@
         <v>174</v>
       </c>
       <c r="B239" s="3" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="C239" s="52" t="s">
         <v>572</v>
@@ -25484,10 +25477,10 @@
         <v>200</v>
       </c>
       <c r="E239" s="13" t="s">
+        <v>1713</v>
+      </c>
+      <c r="F239" s="55" t="s">
         <v>1714</v>
-      </c>
-      <c r="F239" s="55" t="s">
-        <v>1715</v>
       </c>
       <c r="G239" s="19" t="s">
         <v>1079</v>
@@ -25513,7 +25506,7 @@
         <v>516</v>
       </c>
       <c r="F240" s="55" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="G240" s="19" t="s">
         <v>1080</v>
@@ -25553,10 +25546,10 @@
         <v>177</v>
       </c>
       <c r="B242" s="3" t="s">
+        <v>1716</v>
+      </c>
+      <c r="C242" s="52" t="s">
         <v>1717</v>
-      </c>
-      <c r="C242" s="52" t="s">
-        <v>1718</v>
       </c>
       <c r="D242" s="6" t="s">
         <v>24</v>
@@ -25579,10 +25572,10 @@
         <v>178</v>
       </c>
       <c r="B243" s="33" t="s">
+        <v>1718</v>
+      </c>
+      <c r="C243" s="54" t="s">
         <v>1719</v>
-      </c>
-      <c r="C243" s="54" t="s">
-        <v>1720</v>
       </c>
       <c r="D243" s="33" t="s">
         <v>204</v>
@@ -25608,7 +25601,7 @@
         <v>361</v>
       </c>
       <c r="C244" s="51" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D244" s="11" t="s">
         <v>1084</v>
@@ -25660,7 +25653,7 @@
         <v>1231</v>
       </c>
       <c r="C246" s="54" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D246" s="33" t="s">
         <v>369</v>
@@ -25712,16 +25705,16 @@
         <v>1485</v>
       </c>
       <c r="C248" s="54" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D248" s="33" t="s">
         <v>371</v>
       </c>
       <c r="E248" s="34" t="s">
+        <v>1724</v>
+      </c>
+      <c r="F248" s="60" t="s">
         <v>1725</v>
-      </c>
-      <c r="F248" s="60" t="s">
-        <v>1726</v>
       </c>
       <c r="G248" s="35" t="s">
         <v>1089</v>
@@ -25738,7 +25731,7 @@
         <v>1232</v>
       </c>
       <c r="C249" s="51" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D249" s="11" t="s">
         <v>114</v>
@@ -25904,10 +25897,10 @@
         <v>188</v>
       </c>
       <c r="B256" s="3" t="s">
+        <v>1727</v>
+      </c>
+      <c r="C256" s="52" t="s">
         <v>1728</v>
-      </c>
-      <c r="C256" s="52" t="s">
-        <v>1729</v>
       </c>
       <c r="D256" s="3" t="s">
         <v>63</v>
@@ -25959,16 +25952,16 @@
         <v>216</v>
       </c>
       <c r="C258" s="52" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D258" s="3" t="s">
         <v>217</v>
       </c>
       <c r="E258" s="13" t="s">
+        <v>1730</v>
+      </c>
+      <c r="F258" s="55" t="s">
         <v>1731</v>
-      </c>
-      <c r="F258" s="55" t="s">
-        <v>1732</v>
       </c>
       <c r="G258" s="19" t="s">
         <v>1099</v>
@@ -25991,10 +25984,10 @@
         <v>63</v>
       </c>
       <c r="E259" s="13" t="s">
+        <v>1732</v>
+      </c>
+      <c r="F259" s="75" t="s">
         <v>1733</v>
-      </c>
-      <c r="F259" s="75" t="s">
-        <v>1734</v>
       </c>
       <c r="G259" s="19" t="s">
         <v>1100</v>
@@ -26008,10 +26001,10 @@
         <v>192</v>
       </c>
       <c r="B260" s="3" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="C260" s="52" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D260" s="3" t="s">
         <v>1101</v>
@@ -26037,7 +26030,7 @@
         <v>1235</v>
       </c>
       <c r="C261" s="52" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D261" s="3" t="s">
         <v>218</v>
@@ -26121,10 +26114,10 @@
         <v>206</v>
       </c>
       <c r="E264" s="14" t="s">
+        <v>1735</v>
+      </c>
+      <c r="F264" s="84" t="s">
         <v>1736</v>
-      </c>
-      <c r="F264" s="84" t="s">
-        <v>1737</v>
       </c>
       <c r="G264" s="18" t="s">
         <v>1106</v>
@@ -26141,7 +26134,7 @@
         <v>1107</v>
       </c>
       <c r="C265" s="51" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D265" s="11" t="s">
         <v>207</v>
@@ -26167,7 +26160,7 @@
         <v>1109</v>
       </c>
       <c r="C266" s="51" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D266" s="11" t="s">
         <v>207</v>
@@ -26216,10 +26209,10 @@
         <v>183</v>
       </c>
       <c r="B268" s="3" t="s">
+        <v>1739</v>
+      </c>
+      <c r="C268" s="52" t="s">
         <v>1740</v>
-      </c>
-      <c r="C268" s="52" t="s">
-        <v>1741</v>
       </c>
       <c r="D268" s="6" t="s">
         <v>24</v>
@@ -26483,7 +26476,7 @@
         <v>460</v>
       </c>
       <c r="F278" s="53" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="G278" s="18" t="s">
         <v>1122</v>
@@ -26532,10 +26525,10 @@
         <v>380</v>
       </c>
       <c r="E280" s="14" t="s">
+        <v>1742</v>
+      </c>
+      <c r="F280" s="53" t="s">
         <v>1743</v>
-      </c>
-      <c r="F280" s="53" t="s">
-        <v>1744</v>
       </c>
       <c r="G280" s="18" t="s">
         <v>1125</v>
@@ -26626,7 +26619,7 @@
         <v>386</v>
       </c>
       <c r="C284" s="51" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D284" s="11" t="s">
         <v>387</v>
@@ -26652,7 +26645,7 @@
         <v>1243</v>
       </c>
       <c r="C285" s="51" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D285" s="11" t="s">
         <v>355</v>
@@ -26678,7 +26671,7 @@
         <v>388</v>
       </c>
       <c r="C286" s="51" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D286" s="11" t="s">
         <v>382</v>
@@ -26730,7 +26723,7 @@
         <v>373</v>
       </c>
       <c r="C288" s="56" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D288" s="6"/>
       <c r="E288" s="23"/>
@@ -26750,7 +26743,7 @@
         <v>390</v>
       </c>
       <c r="C289" s="54" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D289" s="33" t="s">
         <v>391</v>
@@ -26811,7 +26804,7 @@
         <v>1564</v>
       </c>
       <c r="F291" s="53" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="G291" s="18" t="s">
         <v>1137</v>
@@ -26854,7 +26847,7 @@
         <v>1245</v>
       </c>
       <c r="C293" s="54" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D293" s="33" t="s">
         <v>223</v>
@@ -26906,16 +26899,16 @@
         <v>1581</v>
       </c>
       <c r="C295" s="54" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D295" s="33" t="s">
         <v>221</v>
       </c>
       <c r="E295" s="34" t="s">
+        <v>1752</v>
+      </c>
+      <c r="F295" s="60" t="s">
         <v>1753</v>
-      </c>
-      <c r="F295" s="60" t="s">
-        <v>1754</v>
       </c>
       <c r="G295" s="35" t="s">
         <v>1141</v>
@@ -26984,7 +26977,7 @@
         <v>1246</v>
       </c>
       <c r="C298" s="54" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D298" s="33" t="s">
         <v>395</v>
@@ -27036,7 +27029,7 @@
         <v>1248</v>
       </c>
       <c r="C300" s="54" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D300" s="33" t="s">
         <v>397</v>
@@ -27246,10 +27239,10 @@
         <v>77</v>
       </c>
       <c r="E308" s="13" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="F308" s="75" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="G308" s="19" t="s">
         <v>1154</v>
@@ -27367,19 +27360,19 @@
         <v>202</v>
       </c>
       <c r="B313" s="33" t="s">
+        <v>1757</v>
+      </c>
+      <c r="C313" s="54" t="s">
         <v>1758</v>
-      </c>
-      <c r="C313" s="54" t="s">
-        <v>1759</v>
       </c>
       <c r="D313" s="33" t="s">
         <v>224</v>
       </c>
       <c r="E313" s="34" t="s">
+        <v>1787</v>
+      </c>
+      <c r="F313" s="60" t="s">
         <v>1788</v>
-      </c>
-      <c r="F313" s="60" t="s">
-        <v>1789</v>
       </c>
       <c r="G313" s="35" t="s">
         <v>1159</v>
@@ -27402,10 +27395,10 @@
         <v>226</v>
       </c>
       <c r="E314" s="14" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F314" s="53" t="s">
         <v>1760</v>
-      </c>
-      <c r="F314" s="53" t="s">
-        <v>1761</v>
       </c>
       <c r="G314" s="18" t="s">
         <v>1160</v>
@@ -27607,10 +27600,10 @@
         <v>366</v>
       </c>
       <c r="B322" s="33" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="C322" s="54" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D322" s="33" t="s">
         <v>355</v>
@@ -27714,7 +27707,7 @@
         <v>431</v>
       </c>
       <c r="C326" s="52" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D326" s="3" t="s">
         <v>406</v>
@@ -27844,7 +27837,7 @@
         <v>426</v>
       </c>
       <c r="C331" s="54" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D331" s="33" t="s">
         <v>427</v>
@@ -27879,7 +27872,7 @@
         <v>476</v>
       </c>
       <c r="F332" s="63" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="G332" s="19" t="s">
         <v>1179</v>
@@ -27919,7 +27912,7 @@
         <v>370</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="C334" s="52" t="s">
         <v>1622</v>
@@ -28002,10 +27995,10 @@
         <v>24</v>
       </c>
       <c r="E337" s="13" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="F337" s="55" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="G337" s="19" t="s">
         <v>1184</v>
@@ -28045,10 +28038,10 @@
         <v>219</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="C339" s="52" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D339" s="3" t="s">
         <v>238</v>
@@ -28071,19 +28064,19 @@
         <v>211</v>
       </c>
       <c r="B340" s="33" t="s">
+        <v>1768</v>
+      </c>
+      <c r="C340" s="54" t="s">
         <v>1769</v>
-      </c>
-      <c r="C340" s="54" t="s">
-        <v>1770</v>
       </c>
       <c r="D340" s="33" t="s">
         <v>231</v>
       </c>
       <c r="E340" s="34" t="s">
+        <v>1789</v>
+      </c>
+      <c r="F340" s="60" t="s">
         <v>1790</v>
-      </c>
-      <c r="F340" s="60" t="s">
-        <v>1791</v>
       </c>
       <c r="G340" s="35" t="s">
         <v>1187</v>
@@ -28106,10 +28099,10 @@
         <v>232</v>
       </c>
       <c r="E341" s="34" t="s">
+        <v>1770</v>
+      </c>
+      <c r="F341" s="60" t="s">
         <v>1771</v>
-      </c>
-      <c r="F341" s="60" t="s">
-        <v>1772</v>
       </c>
       <c r="G341" s="35" t="s">
         <v>1188</v>
@@ -28132,10 +28125,10 @@
         <v>114</v>
       </c>
       <c r="E342" s="34" t="s">
+        <v>1776</v>
+      </c>
+      <c r="F342" s="60" t="s">
         <v>1777</v>
-      </c>
-      <c r="F342" s="60" t="s">
-        <v>1778</v>
       </c>
       <c r="G342" s="35" t="s">
         <v>1189</v>
@@ -28178,7 +28171,7 @@
         <v>234</v>
       </c>
       <c r="C344" s="52" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D344" s="3" t="s">
         <v>1569</v>
@@ -28210,10 +28203,10 @@
         <v>1572</v>
       </c>
       <c r="E345" s="42" t="s">
+        <v>1779</v>
+      </c>
+      <c r="F345" s="78" t="s">
         <v>1780</v>
-      </c>
-      <c r="F345" s="78" t="s">
-        <v>1781</v>
       </c>
       <c r="G345" s="19" t="s">
         <v>1192</v>
@@ -28230,7 +28223,7 @@
         <v>432</v>
       </c>
       <c r="C346" s="52" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D346" s="3" t="s">
         <v>406</v>
@@ -28256,7 +28249,7 @@
         <v>1259</v>
       </c>
       <c r="C347" s="52" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D347" s="3" t="s">
         <v>433</v>
@@ -28334,7 +28327,7 @@
         <v>240</v>
       </c>
       <c r="C350" s="52" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D350" s="3" t="s">
         <v>241</v>
@@ -28383,19 +28376,19 @@
         <v>222</v>
       </c>
       <c r="B352" s="33" t="s">
+        <v>1785</v>
+      </c>
+      <c r="C352" s="54" t="s">
         <v>1786</v>
-      </c>
-      <c r="C352" s="54" t="s">
-        <v>1787</v>
       </c>
       <c r="D352" s="33" t="s">
         <v>243</v>
       </c>
       <c r="E352" s="34" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F352" s="60" t="s">
         <v>1792</v>
-      </c>
-      <c r="F352" s="60" t="s">
-        <v>1793</v>
       </c>
       <c r="G352" s="35" t="s">
         <v>1199</v>
@@ -28418,10 +28411,10 @@
         <v>245</v>
       </c>
       <c r="E353" s="34" t="s">
+        <v>1793</v>
+      </c>
+      <c r="F353" s="60" t="s">
         <v>1794</v>
-      </c>
-      <c r="F353" s="60" t="s">
-        <v>1795</v>
       </c>
       <c r="G353" s="35" t="s">
         <v>1200</v>
@@ -28457,10 +28450,10 @@
         <v>225</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="C355" s="52" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="D355" s="3" t="s">
         <v>247</v>
@@ -28492,10 +28485,10 @@
         <v>1136</v>
       </c>
       <c r="E356" s="34" t="s">
+        <v>1797</v>
+      </c>
+      <c r="F356" s="60" t="s">
         <v>1798</v>
-      </c>
-      <c r="F356" s="60" t="s">
-        <v>1799</v>
       </c>
       <c r="G356" s="35" t="s">
         <v>1203</v>
@@ -28512,7 +28505,7 @@
         <v>234</v>
       </c>
       <c r="C357" s="52" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D357" s="3" t="s">
         <v>1573</v>
@@ -28535,7 +28528,7 @@
         <v>229</v>
       </c>
       <c r="B358" s="3" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="C358" s="52" t="s">
         <v>741</v>
@@ -28561,7 +28554,7 @@
         <v>232</v>
       </c>
       <c r="B359" s="3" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="C359" s="52" t="s">
         <v>741</v>
@@ -28601,7 +28594,7 @@
         <v>1207</v>
       </c>
       <c r="H360" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
     </row>
     <row r="361" spans="1:8" s="36" customFormat="1" ht="45" x14ac:dyDescent="0.25">
@@ -28618,10 +28611,10 @@
         <v>114</v>
       </c>
       <c r="E361" s="34" t="s">
+        <v>1802</v>
+      </c>
+      <c r="F361" s="60" t="s">
         <v>1803</v>
-      </c>
-      <c r="F361" s="60" t="s">
-        <v>1804</v>
       </c>
       <c r="G361" s="35" t="s">
         <v>1208</v>
@@ -28664,16 +28657,16 @@
         <v>274</v>
       </c>
       <c r="C363" s="54" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D363" s="33" t="s">
         <v>275</v>
       </c>
       <c r="E363" s="34" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="F363" s="60" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="G363" s="35" t="s">
         <v>1210</v>
@@ -28696,10 +28689,10 @@
         <v>277</v>
       </c>
       <c r="E364" s="34" t="s">
+        <v>1806</v>
+      </c>
+      <c r="F364" s="60" t="s">
         <v>1807</v>
-      </c>
-      <c r="F364" s="60" t="s">
-        <v>1808</v>
       </c>
       <c r="G364" s="35" t="s">
         <v>1211</v>
@@ -28713,19 +28706,19 @@
         <v>234</v>
       </c>
       <c r="B365" s="33" t="s">
+        <v>1808</v>
+      </c>
+      <c r="C365" s="54" t="s">
         <v>1809</v>
-      </c>
-      <c r="C365" s="54" t="s">
-        <v>1810</v>
       </c>
       <c r="D365" s="33" t="s">
         <v>255</v>
       </c>
       <c r="E365" s="34" t="s">
+        <v>1791</v>
+      </c>
+      <c r="F365" s="60" t="s">
         <v>1792</v>
-      </c>
-      <c r="F365" s="60" t="s">
-        <v>1793</v>
       </c>
       <c r="G365" s="35" t="s">
         <v>1212</v>
@@ -28748,10 +28741,10 @@
         <v>114</v>
       </c>
       <c r="E366" s="34" t="s">
+        <v>1810</v>
+      </c>
+      <c r="F366" s="60" t="s">
         <v>1811</v>
-      </c>
-      <c r="F366" s="60" t="s">
-        <v>1812</v>
       </c>
       <c r="G366" s="35" t="s">
         <v>1213</v>
@@ -28790,16 +28783,16 @@
         <v>258</v>
       </c>
       <c r="C368" s="54" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D368" s="33" t="s">
         <v>1136</v>
       </c>
       <c r="E368" s="34" t="s">
+        <v>1812</v>
+      </c>
+      <c r="F368" s="60" t="s">
         <v>1813</v>
-      </c>
-      <c r="F368" s="60" t="s">
-        <v>1814</v>
       </c>
       <c r="G368" s="35" t="s">
         <v>1215</v>
@@ -28822,10 +28815,10 @@
         <v>260</v>
       </c>
       <c r="E369" s="34" t="s">
+        <v>1814</v>
+      </c>
+      <c r="F369" s="76" t="s">
         <v>1815</v>
-      </c>
-      <c r="F369" s="76" t="s">
-        <v>1816</v>
       </c>
       <c r="G369" s="35" t="s">
         <v>1216</v>
@@ -28868,16 +28861,16 @@
         <v>262</v>
       </c>
       <c r="C371" s="52" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D371" s="3" t="s">
         <v>263</v>
       </c>
       <c r="E371" s="13" t="s">
+        <v>1817</v>
+      </c>
+      <c r="F371" s="55" t="s">
         <v>1818</v>
-      </c>
-      <c r="F371" s="55" t="s">
-        <v>1819</v>
       </c>
       <c r="G371" s="19" t="s">
         <v>1218</v>
@@ -28926,10 +28919,10 @@
         <v>267</v>
       </c>
       <c r="E373" s="13" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="F373" s="55" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="G373" s="19" t="s">
         <v>1220</v>
@@ -28943,19 +28936,19 @@
         <v>245</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="C374" s="52" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D374" s="6" t="s">
         <v>24</v>
       </c>
       <c r="E374" s="13" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="F374" s="55" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="G374" s="19" t="s">
         <v>1221</v>
@@ -28998,7 +28991,7 @@
         <v>1262</v>
       </c>
       <c r="C376" s="54" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D376" s="33" t="s">
         <v>266</v>
@@ -29024,7 +29017,7 @@
         <v>270</v>
       </c>
       <c r="C377" s="52" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D377" s="3" t="s">
         <v>268</v>
@@ -29050,7 +29043,7 @@
         <v>271</v>
       </c>
       <c r="C378" s="52" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D378" s="3" t="s">
         <v>269</v>
@@ -29076,7 +29069,7 @@
         <v>272</v>
       </c>
       <c r="C379" s="52" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D379" s="3" t="s">
         <v>273</v>
@@ -29099,19 +29092,19 @@
         <v>249</v>
       </c>
       <c r="B380" s="33" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="C380" s="54" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D380" s="33" t="s">
         <v>338</v>
       </c>
       <c r="E380" s="34" t="s">
+        <v>1828</v>
+      </c>
+      <c r="F380" s="60" t="s">
         <v>1829</v>
-      </c>
-      <c r="F380" s="60" t="s">
-        <v>1830</v>
       </c>
       <c r="G380" s="35" t="s">
         <v>1227</v>

</xml_diff>